<commit_message>
Correccion 06 - Bocaccio/Ledesma OK
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -176,7 +176,7 @@
       <name val="Aptos narrow"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +207,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -287,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -310,6 +316,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -319,10 +331,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -618,12 +627,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:4" ht="105" customHeight="1" thickBot="1">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1">
       <c r="B5" s="1" t="s">
@@ -640,10 +649,10 @@
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -662,10 +671,10 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -673,10 +682,10 @@
       <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -695,10 +704,10 @@
       <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -706,7 +715,7 @@
       <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="4"/>
@@ -715,10 +724,10 @@
       <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -726,10 +735,10 @@
       <c r="B14" s="3">
         <v>9</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -737,10 +746,10 @@
       <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -748,10 +757,10 @@
       <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -759,10 +768,10 @@
       <c r="B17" s="3">
         <v>12</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -770,10 +779,10 @@
       <c r="B18" s="3">
         <v>13</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -792,10 +801,10 @@
       <c r="B20" s="3">
         <v>15</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -803,10 +812,10 @@
       <c r="B21" s="3">
         <v>16</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="8" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion 06 - Tengo que terminar devolucion Cecilia coronel
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC71D3-BD2E-4E0B-AA6A-BBD1A43254A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -138,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +323,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -329,9 +333,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,28 +614,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="3" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B4" s="10" t="s">
+    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -645,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="6" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -656,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -667,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -678,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="9" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -689,7 +690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="10" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>5</v>
       </c>
@@ -700,18 +701,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="11" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="12" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>7</v>
       </c>
@@ -720,7 +721,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="13" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -731,7 +732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="14" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -742,18 +743,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="15" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="16" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -764,7 +765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="17" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>12</v>
       </c>
@@ -775,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="18" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>13</v>
       </c>
@@ -786,7 +787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="19" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>14</v>
       </c>
@@ -797,7 +798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="20" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>15</v>
       </c>
@@ -808,7 +809,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="21" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>16</v>
       </c>
@@ -819,14 +820,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="22" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>17</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="23" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>18</v>
       </c>
@@ -835,7 +836,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="24" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>19</v>
       </c>
@@ -844,7 +845,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="25" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>20</v>
       </c>
@@ -853,7 +854,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
+    <row r="26" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="6"/>

</xml_diff>

<commit_message>
Correccion 06 - Estoy en matias Pinte
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC71D3-BD2E-4E0B-AA6A-BBD1A43254A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -139,8 +138,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,28 +613,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -657,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -668,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -679,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -690,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B10" s="3">
         <v>5</v>
       </c>
@@ -701,7 +700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B11" s="3">
         <v>6</v>
       </c>
@@ -712,7 +711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B12" s="3">
         <v>7</v>
       </c>
@@ -721,7 +720,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -732,7 +731,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -743,7 +742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -754,7 +753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -765,7 +764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B17" s="3">
         <v>12</v>
       </c>
@@ -776,18 +775,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B18" s="3">
         <v>13</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B19" s="3">
         <v>14</v>
       </c>
@@ -798,18 +797,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B20" s="3">
         <v>15</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B21" s="3">
         <v>16</v>
       </c>
@@ -820,14 +819,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B22" s="3">
         <v>17</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B23" s="3">
         <v>18</v>
       </c>
@@ -836,7 +835,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B24" s="3">
         <v>19</v>
       </c>
@@ -845,7 +844,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B25" s="3">
         <v>20</v>
       </c>
@@ -854,7 +853,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="35.25" customHeight="1" thickBot="1">
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="6"/>

</xml_diff>

<commit_message>
Correccion - Tatiana Iglesias y Mariani - Terminado ok
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CE7AD1-5A3A-4D3F-8638-2543BC004A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -322,6 +323,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -329,9 +333,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,11 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -628,11 +629,11 @@
   <sheetData>
     <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1">
       <c r="B5" s="1" t="s">
@@ -738,7 +739,7 @@
       <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -757,10 +758,10 @@
       <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -812,10 +813,10 @@
       <c r="B21" s="3">
         <v>16</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion 06 - Diaz Facundo/ Mendoza Diego terminado OK
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CE7AD1-5A3A-4D3F-8638-2543BC004A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F28F64-27EE-4BD5-AFBC-CE0C447859C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -769,10 +769,10 @@
       <c r="B17" s="3">
         <v>12</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion 06 - De Oliveira / Teves terminado OK
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F28F64-27EE-4BD5-AFBC-CE0C447859C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -139,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -614,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -725,10 +724,10 @@
       <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion - Terminado en Eiriz Nicolas OK hasta 27/8
</commit_message>
<xml_diff>
--- a/Desafios/06/pair programming.xlsx
+++ b/Desafios/06/pair programming.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17BA7D7-40B8-4C26-A6AE-335C8C778674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -176,7 +177,7 @@
       <name val="Aptos narrow"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,12 +204,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -293,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,10 +314,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="C8:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -628,11 +620,11 @@
   <sheetData>
     <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="2:4" ht="36" customHeight="1" thickBot="1">
       <c r="B5" s="1" t="s">
@@ -671,10 +663,10 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -682,10 +674,10 @@
       <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -704,10 +696,10 @@
       <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -715,7 +707,7 @@
       <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="4"/>
@@ -724,10 +716,10 @@
       <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -735,10 +727,10 @@
       <c r="B14" s="3">
         <v>9</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -746,10 +738,10 @@
       <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -757,10 +749,10 @@
       <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -768,10 +760,10 @@
       <c r="B17" s="3">
         <v>12</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -779,10 +771,10 @@
       <c r="B18" s="3">
         <v>13</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -801,10 +793,10 @@
       <c r="B20" s="3">
         <v>15</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -812,10 +804,10 @@
       <c r="B21" s="3">
         <v>16</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>